<commit_message>
dataexporter add postfix and use staticdata in project
</commit_message>
<xml_diff>
--- a/StaticData/Actor.xlsx
+++ b/StaticData/Actor.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\MonMoose\StaticData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\MonMoose\StaticData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7DC17B-E2C3-4554-8AE5-61A84DC68758}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225"/>
   </bookViews>
   <sheets>
     <sheet name="Actor" sheetId="1" r:id="rId1"/>
-    <sheet name="EActorType" sheetId="2" r:id="rId2"/>
+    <sheet name="EActorClassType" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Data</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,10 +91,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>EActorType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Actor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,18 +131,37 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Warrior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>EActorClassType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Warrior</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PrefabPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exported/Actor/001/Prefabs/Actor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,31 +488,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.25" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
     <col min="6" max="6" width="14.375" customWidth="1"/>
+    <col min="7" max="7" width="32.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -517,8 +532,11 @@
       <c r="F2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -537,8 +555,11 @@
       <c r="F3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -546,7 +567,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -557,30 +578,36 @@
       <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
       <c r="D8">
         <v>500</v>
       </c>
@@ -589,20 +616,24 @@
       </c>
       <c r="F8">
         <v>1100</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF3D370-A925-4088-B67B-45C083EB3752}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -612,7 +643,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>27</v>
@@ -620,10 +651,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -631,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -639,7 +670,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -647,7 +678,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -655,7 +686,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -663,7 +694,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -671,7 +702,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -679,7 +710,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multi grid actor path finder
</commit_message>
<xml_diff>
--- a/StaticData/Actor.xlsx
+++ b/StaticData/Actor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\MonMoose\StaticData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC0DA23-E62E-4782-BB67-1DFBFF24B3D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774162FF-865C-47A1-9432-2A347257A34E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Actor" sheetId="1" r:id="rId1"/>
     <sheet name="EActorClassType" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Data</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -153,6 +153,26 @@
   </si>
   <si>
     <t>Exported/Actor/001/Prefabs/Actor</t>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Int32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exported/Actor/001/Prefabs/Actor2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exported/Actor/001/Prefabs/Actor3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -486,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -502,7 +522,7 @@
     <col min="7" max="7" width="32.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +530,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -532,8 +552,11 @@
       <c r="G2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -555,8 +578,11 @@
       <c r="G3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -578,24 +604,27 @@
       <c r="G4" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -616,6 +645,61 @@
       </c>
       <c r="G8" t="s">
         <v>31</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>500</v>
+      </c>
+      <c r="E9">
+        <v>1100</v>
+      </c>
+      <c r="F9">
+        <v>1100</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>500</v>
+      </c>
+      <c r="E10">
+        <v>1100</v>
+      </c>
+      <c r="F10">
+        <v>1100</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>